<commit_message>
reduce excel generator boiler code
</commit_message>
<xml_diff>
--- a/backend/excel_sheets/extracted_data_1758268326704.xlsx
+++ b/backend/excel_sheets/extracted_data_1758268326704.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,112 +591,112 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Summary of Product Characteristics</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Awiqli</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>insulin icodec</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>700 units/mL</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Solution for injection in pre-filled pen</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Subcutaneous use</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Treatment of diabetes mellitus in adults</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Once-weekly subcutaneous administration, dose range 10-700 units per injection</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Hypersensitivity to the active substance or to any of the excipients</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Risk of hypoglycaemia, hypersensitivity reactions, and immune system disorders</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Novo Nordisk A/S</t>
         </is>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>EU/1/24/1815/001, EU/1/24/1815/002, EU/1/24/1815/003, EU/1/24/1815/004, EU/1/24/1815/005, EU/1/24/1815/006, EU/1/24/1815/007, EU/1/24/1815/008, EU/1/24/1815/009, EU/1/24/1815/010, EU/1/24/1815/011, EU/1/24/1815/012, EU/1/24/1815/013, EU/1/24/1815/014</t>
         </is>
       </c>
       <c r="M2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>17 May 2024</t>
         </is>
       </c>
       <c r="N2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>"Date of Latest Renewal": "Not found",</t>
         </is>
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>3 years</t>
         </is>
       </c>
       <c r="P2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Store in a refrigerator (2 °C - 8 °C), do not freeze, keep the cap on the pen to protect from light</t>
         </is>
       </c>
       <c r="Q2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Pre-filled pen containing 700 units of insulin icodec in 1 mL solution, 1.5 mL solution, or 3 mL solution</t>
         </is>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Prescription only</t>
         </is>
       </c>
       <c r="S2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>A10AE07</t>
         </is>
       </c>
       <c r="T2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Novo Nordisk A/S</t>
         </is>
       </c>
       <c r="U2" s="2" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Glycerol, metacresol, phenol, zinc acetate, sodium chloride, hydrochloric acid, sodium hydroxide, and water for injections</t>
         </is>
       </c>
       <c r="V2" s="2" t="inlineStr">
         <is>
-          <t>https://graph.microsoft.com/v1.0/sites/slickbitai.sharepoint.com,b749c6f0-ede8-48b2-9420-ce94ca741683,876dc7c6-5b74-44d2-9d5c-a40b9e5cbf21/drive/root:/application_test1</t>
+          <t>awiqli-epar-product-information_en.pdf</t>
         </is>
       </c>
       <c r="W2" s="2" t="inlineStr">
@@ -708,115 +708,232 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Summary of Product Characteristics</t>
+          <t>Not found</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> https://graph.microsoft.com/v1.0/sites/slickbitai.sharepoint.com,b749c6f0-ede8-48b2-9420-ce94ca741683,876dc7c6-5b74-44d2-9d5c-a40b9e5cbf21/drive/root:/application_test1</t>
+        </is>
+      </c>
+      <c r="W3" s="2" t="inlineStr">
+        <is>
+          <t>1758268326704</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Summary of Product Characteristics, SmPC, Product Information</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
           <t>Awiqli</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>insulin icodec</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>700 units/mL</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Solution for injection in pre-filled pen</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Subcutaneous use</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Treatment of diabetes mellitus in adults</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Once-weekly subcutaneous administration, dose range 10-700 units per injection</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>Once-weekly subcutaneous administration, dose adjusted based on fasting plasma glucose</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>Hypersensitivity to the active substance or to any of the excipients</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>Risk of hypoglycaemia, hypersensitivity reactions, and immune system disorders</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>Risk of hypoglycaemia,Switch between other insulins and insulin icodec should be done under medical supervision</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
         <is>
           <t>Novo Nordisk A/S</t>
         </is>
       </c>
-      <c r="L3" s="2" t="inlineStr">
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>EU/1/24/1815/001, EU/1/24/1815/002, EU/1/24/1815/003, EU/1/24/1815/004, EU/1/24/1815/005, EU/1/24/1815/006, EU/1/24/1815/007, EU/1/24/1815/008, EU/1/24/1815/009, EU/1/24/1815/010, EU/1/24/1815/011, EU/1/24/1815/012, EU/1/24/1815/013, EU/1/24/1815/014</t>
         </is>
       </c>
-      <c r="M3" s="2" t="inlineStr">
+      <c r="M4" s="2" t="inlineStr">
         <is>
           <t>17 May 2024</t>
         </is>
       </c>
-      <c r="N3" s="2" t="inlineStr">
+      <c r="N4" s="2" t="inlineStr">
         <is>
           <t>"Date of Latest Renewal": "Not found",</t>
         </is>
       </c>
-      <c r="O3" s="2" t="inlineStr">
-        <is>
-          <t>3 years</t>
-        </is>
-      </c>
-      <c r="P3" s="2" t="inlineStr">
-        <is>
-          <t>Store in a refrigerator (2 °C - 8 °C), do not freeze, keep the cap on the pen to protect from light</t>
-        </is>
-      </c>
-      <c r="Q3" s="2" t="inlineStr">
-        <is>
-          <t>Pre-filled pen containing 700 units of insulin icodec in 1 mL solution, 1.5 mL solution, or 3 mL solution</t>
-        </is>
-      </c>
-      <c r="R3" s="2" t="inlineStr">
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>3 years, After first opening or carried as a spare, the medicinal product may be stored for a maximum of 12 weeks</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
+        <is>
+          <t>Store in a refrigerator (2°C - 8°C), Do not freeze, Keep the cap on the pen in order to protect from light</t>
+        </is>
+      </c>
+      <c r="Q4" s="2" t="inlineStr">
+        <is>
+          <t>1 mL solution contains 700 units of insulin icodec, Each pre-filled pen contains 700 units of insulin icodec in 1 mL solution, Each pre-filled pen contains 1,050 units of insulin icodec in 1.5 mL solution, Each pre-filled pen contains 2,100 units of insulin icodec in 3 mL solution</t>
+        </is>
+      </c>
+      <c r="R4" s="2" t="inlineStr">
         <is>
           <t>Prescription only</t>
         </is>
       </c>
-      <c r="S3" s="2" t="inlineStr">
+      <c r="S4" s="2" t="inlineStr">
         <is>
           <t>A10AE07</t>
         </is>
       </c>
-      <c r="T3" s="2" t="inlineStr">
+      <c r="T4" s="2" t="inlineStr">
         <is>
           <t>Novo Nordisk A/S</t>
         </is>
       </c>
-      <c r="U3" s="2" t="inlineStr">
-        <is>
-          <t>Glycerol, metacresol, phenol, zinc acetate, sodium chloride, hydrochloric acid, sodium hydroxide, and water for injections</t>
-        </is>
-      </c>
-      <c r="V3" s="2" t="inlineStr">
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>Glycerol, Metacresol, Phenol, Zinc acetate, Sodium chloride, Hydrochloric acid, Sodium hydroxide, Water for injections</t>
+        </is>
+      </c>
+      <c r="V4" s="2" t="inlineStr">
         <is>
           <t>awiqli-epar-product-information_en.pdf</t>
         </is>
       </c>
-      <c r="W3" s="2" t="inlineStr">
+      <c r="W4" s="2" t="inlineStr">
         <is>
           <t>1758268326704</t>
         </is>

</xml_diff>